<commit_message>
Updated burndown chart and removed remnants of the past
</commit_message>
<xml_diff>
--- a/Sprint 3 Burndown Chart.xlsx
+++ b/Sprint 3 Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taylo\Desktop\College Folder\Spring 2022\CSE 3902\Sprint 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AE08972-EEA2-46FB-96D0-357A5EA0BCD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4643D3C4-4206-49CA-875E-C3FC70D88700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F41D13B3-3180-4E80-BADE-112D0D5566D0}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Adjusted sprites. Code cleanup</t>
+  </si>
+  <si>
+    <t>Finished basement as well as miscellainous items</t>
   </si>
 </sst>
 </file>
@@ -162,11 +165,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Sprint</a:t>
+              <a:t>Sprint 3</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> 3 Burndown Chart</a:t>
+              <a:t> Burndown Chart</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -306,20 +309,10 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$A$2:$B$10</c15:sqref>
-                  </c15:fullRef>
-                  <c15:levelRef>
-                    <c15:sqref>Sheet1!$A$2:$A$10</c15:sqref>
-                  </c15:levelRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Sheet1!$A$2:$A$10</c:f>
+              <c:f>Sheet1!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>44617</c:v>
                 </c:pt>
@@ -346,16 +339,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>44630</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44631</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$10</c:f>
+              <c:f>Sheet1!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -382,13 +378,16 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9399-4A78-ABA7-E64A92B9F68C}"/>
+              <c16:uniqueId val="{00000000-49A4-4A4C-AAC7-EB5DD4D4F7C1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -403,11 +402,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="990974191"/>
-        <c:axId val="990991663"/>
+        <c:axId val="457324864"/>
+        <c:axId val="457325280"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="990974191"/>
+        <c:axId val="457324864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,19 +433,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Dates</a:t>
+                  <a:t>Date</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.47221412948381453"/>
-              <c:y val="0.87405074365704283"/>
-            </c:manualLayout>
-          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -513,14 +504,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990991663"/>
+        <c:crossAx val="457325280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="990991663"/>
+        <c:axId val="457325280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -561,8 +552,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Percent of Tasks Left</a:t>
+                  <a:t>Percent of tasks</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> done</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -626,7 +622,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="990974191"/>
+        <c:crossAx val="457324864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1223,22 +1219,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>23812</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>328612</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BD12CC3-3914-49AB-BA08-F028D22F7C9A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4593E30-902B-40B4-99AA-C0AAED439BC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1556,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{603FE3B5-6C28-4BC9-B9A7-9592872FAE5E}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1678,6 +1674,17 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>44631</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>